<commit_message>
update dairy to 02/16
</commit_message>
<xml_diff>
--- a/diaries/diary-Yue Zhang.xlsx
+++ b/diaries/diary-Yue Zhang.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yorkson/Dropbox/SWE 265P/W2020/diaries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yorkson\Dropbox\MSWE-Q2\SWE-265P\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258DA22D-8F3D-2B4D-BB20-D220BB8F9E87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C08646-C81B-4506-BAEC-F9562C70ABC2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41140" yWindow="3860" windowWidth="28800" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="2352" yWindow="3540" windowWidth="23040" windowHeight="12204" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -53,42 +53,18 @@
     <t>Participants</t>
   </si>
   <si>
-    <t>&lt;what day?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what time?&gt;</t>
-  </si>
-  <si>
     <t>Reflection</t>
   </si>
   <si>
-    <t>&lt;as applicable, with whom?&gt;</t>
-  </si>
-  <si>
     <t>Your Overall Mood</t>
   </si>
   <si>
     <t>Goal</t>
   </si>
   <si>
-    <t>&lt;what did you want to accomplish?&gt;</t>
-  </si>
-  <si>
     <t>Achievements</t>
   </si>
   <si>
-    <t>&lt;what did you actually accomplish?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what insight(s) did you gain?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;how did you feel during the activity?&gt;</t>
-  </si>
-  <si>
-    <t>Etc.</t>
-  </si>
-  <si>
     <t>Yue Zhang</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -101,10 +77,6 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>01/11/2020</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>Setting up development environments.  And send a pull request to the repositories.</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -122,6 +94,162 @@
   </si>
   <si>
     <t>N/A</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Review the basic strategies of code understanding</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>I am feeling so so.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>The basic strategies are useful.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Build and read the source code of  JPacMan. Take notes about today's lesson.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finish the homework on project Jpacman.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Read source code. Write reports. Take notes.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>I am feeling happy.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>JPacMan is fun for playing and  reading</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Review the concept of mental models. Take notes about mental model externalization and UML graph.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use intelliJ plugin to draw a uml diagram for Jpacman and explore the source code</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>In good mood.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>This plugin is very useful and I should use it to read source code.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>2:00 - 5:00 PM</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tianlun Li, Zeyu Huang</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Build and read the project we chose.  Discuss what features are we are going to read.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>We decide to use ip filtering and rank evaluation features.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>ElasticSearch is amazing!</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>I am quit excited.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>9:00 - 12:00 PM</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exploring the features we decided to read and document the process well.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reading the source code is a little difficult.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>We fininally completed the goals and wrote a report.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Review the concepts of structural models and behavioral models， UML diagram, Sequence diagram, and call graph.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Take reviewing notes.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>The three diagrams are very helpful for me to read codes.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>7:00-9:00 PM</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get to understand the implement of these two features.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>It' s hard to read such a large project.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>I am feeling unhappy</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>9.00-11.30 PM</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Build and read ElasticSearch engine. Explore the essential features indexing and searching.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Understand the implements of indexing and searching features completely. </t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Draw diagrams and write a report to finish the howework.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Our team became very efficient!</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>I am feeling very happy.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Read and explore the issuses of our project's Github site.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>There're many small problems about this ElasticSearch</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maintaning a big project is not easy</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Just so so.</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -129,7 +257,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,7 +396,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -294,23 +422,32 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="18" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -632,36 +769,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-    </row>
-    <row r="3" spans="1:7" ht="16">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+    </row>
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -670,12 +807,12 @@
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="17">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -683,12 +820,12 @@
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="17">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>20</v>
+      <c r="B5" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -696,12 +833,12 @@
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="17">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>21</v>
+      <c r="B6" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -709,7 +846,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="16">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -718,7 +855,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="16">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -727,7 +864,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="17">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -738,180 +875,276 @@
         <v>6</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="46.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>43841</v>
+      </c>
+      <c r="B10" s="15">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="51">
-      <c r="A10" s="12" t="s">
+      <c r="E10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="46.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>43846</v>
+      </c>
+      <c r="B11" s="15">
+        <v>0.875</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="13">
-        <v>0.94791666666666663</v>
-      </c>
-      <c r="C10" s="12" t="s">
+      <c r="F11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="31.2" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>43848</v>
+      </c>
+      <c r="B12" s="15">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="62.4" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>43853</v>
+      </c>
+      <c r="B13" s="15">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="14" t="s">
+      <c r="E13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="46.8" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>43855</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="46.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>43859</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="62.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>43860</v>
+      </c>
+      <c r="B16" s="15">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17">
-      <c r="A11" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="17">
-      <c r="A12" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="17">
-      <c r="A13" s="12" t="s">
+    <row r="17" spans="1:7" ht="46.8" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>43861</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="46.8" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>43866</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="31.2" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>43877</v>
+      </c>
+      <c r="B19" s="15">
+        <v>0.875</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="14"/>
-    </row>
-    <row r="14" spans="1:7" ht="16">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="14"/>
-    </row>
-    <row r="15" spans="1:7" ht="16">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="14"/>
-    </row>
-    <row r="16" spans="1:7" ht="16">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" ht="16">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="14"/>
-    </row>
-    <row r="18" spans="1:7" ht="16">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="14"/>
-    </row>
-    <row r="19" spans="1:7" ht="16">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="14"/>
-    </row>
-    <row r="20" spans="1:7" ht="16">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="14"/>
-    </row>
-    <row r="21" spans="1:7" ht="16">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="14"/>
-    </row>
-    <row r="22" spans="1:7" ht="16">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="14"/>
-    </row>
-    <row r="23" spans="1:7" ht="16">
+      <c r="D19" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="16"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -920,7 +1153,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:7" ht="16">
+    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -929,7 +1162,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:7" ht="16">
+    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -938,7 +1171,7 @@
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:7" ht="16">
+    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -947,7 +1180,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7" ht="16">
+    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -956,7 +1189,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7" ht="16">
+    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -965,7 +1198,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:7" ht="16">
+    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -974,7 +1207,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7" ht="16">
+    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -983,7 +1216,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:7" ht="16">
+    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -992,7 +1225,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:7" ht="16">
+    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1001,7 +1234,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" spans="1:7" ht="16">
+    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1010,7 +1243,7 @@
       <c r="F33" s="7"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:7" ht="16">
+    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1019,7 +1252,7 @@
       <c r="F34" s="7"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7" ht="16">
+    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1028,7 +1261,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" spans="1:7" ht="16">
+    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1037,7 +1270,7 @@
       <c r="F36" s="7"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" spans="1:7" ht="16">
+    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1046,7 +1279,7 @@
       <c r="F37" s="7"/>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" spans="1:7" ht="16">
+    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1055,7 +1288,7 @@
       <c r="F38" s="7"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" spans="1:7" ht="16">
+    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -1064,7 +1297,7 @@
       <c r="F39" s="7"/>
       <c r="G39" s="8"/>
     </row>
-    <row r="40" spans="1:7" ht="16">
+    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1073,7 +1306,7 @@
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" spans="1:7" ht="16">
+    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1082,7 +1315,7 @@
       <c r="F41" s="7"/>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7" ht="16">
+    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -1091,7 +1324,7 @@
       <c r="F42" s="7"/>
       <c r="G42" s="8"/>
     </row>
-    <row r="43" spans="1:7" ht="16">
+    <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -1100,7 +1333,7 @@
       <c r="F43" s="7"/>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" spans="1:7" ht="16">
+    <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -1109,7 +1342,7 @@
       <c r="F44" s="7"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7" ht="16">
+    <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -1118,7 +1351,7 @@
       <c r="F45" s="7"/>
       <c r="G45" s="8"/>
     </row>
-    <row r="46" spans="1:7" ht="16">
+    <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -1127,7 +1360,7 @@
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" ht="16">
+    <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -1136,7 +1369,7 @@
       <c r="F47" s="7"/>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7" ht="16">
+    <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -1145,7 +1378,7 @@
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="1:7" ht="16">
+    <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -1154,7 +1387,7 @@
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
     </row>
-    <row r="50" spans="1:7" ht="16">
+    <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -1163,7 +1396,7 @@
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7" ht="16">
+    <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -1172,7 +1405,7 @@
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" spans="1:7" ht="16">
+    <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -1181,7 +1414,7 @@
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:7" ht="16">
+    <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1190,7 +1423,7 @@
       <c r="F53" s="7"/>
       <c r="G53" s="8"/>
     </row>
-    <row r="54" spans="1:7" ht="16">
+    <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -1199,7 +1432,7 @@
       <c r="F54" s="7"/>
       <c r="G54" s="8"/>
     </row>
-    <row r="55" spans="1:7" ht="16">
+    <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -1208,7 +1441,7 @@
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7" ht="16">
+    <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -1217,7 +1450,7 @@
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="1:7" ht="16">
+    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -1226,7 +1459,7 @@
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
     </row>
-    <row r="58" spans="1:7" ht="16">
+    <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -1235,7 +1468,7 @@
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
     </row>
-    <row r="59" spans="1:7" ht="16">
+    <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -1244,7 +1477,7 @@
       <c r="F59" s="7"/>
       <c r="G59" s="8"/>
     </row>
-    <row r="60" spans="1:7" ht="16">
+    <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -1253,7 +1486,7 @@
       <c r="F60" s="7"/>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="1:7" ht="16">
+    <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -1262,7 +1495,7 @@
       <c r="F61" s="7"/>
       <c r="G61" s="8"/>
     </row>
-    <row r="62" spans="1:7" ht="16">
+    <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -1271,7 +1504,7 @@
       <c r="F62" s="7"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="1:7" ht="16">
+    <row r="63" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -1280,7 +1513,7 @@
       <c r="F63" s="7"/>
       <c r="G63" s="8"/>
     </row>
-    <row r="64" spans="1:7" ht="16">
+    <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -1289,7 +1522,7 @@
       <c r="F64" s="7"/>
       <c r="G64" s="8"/>
     </row>
-    <row r="65" spans="1:7" ht="16">
+    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -1298,7 +1531,7 @@
       <c r="F65" s="7"/>
       <c r="G65" s="8"/>
     </row>
-    <row r="66" spans="1:7" ht="16">
+    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -1307,7 +1540,7 @@
       <c r="F66" s="7"/>
       <c r="G66" s="8"/>
     </row>
-    <row r="67" spans="1:7" ht="16">
+    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -1316,7 +1549,7 @@
       <c r="F67" s="7"/>
       <c r="G67" s="8"/>
     </row>
-    <row r="68" spans="1:7" ht="16">
+    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -1325,7 +1558,7 @@
       <c r="F68" s="7"/>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="1:7" ht="16">
+    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -1334,7 +1567,7 @@
       <c r="F69" s="7"/>
       <c r="G69" s="8"/>
     </row>
-    <row r="70" spans="1:7" ht="16">
+    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -1343,7 +1576,7 @@
       <c r="F70" s="7"/>
       <c r="G70" s="8"/>
     </row>
-    <row r="71" spans="1:7" ht="16">
+    <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -1352,7 +1585,7 @@
       <c r="F71" s="7"/>
       <c r="G71" s="8"/>
     </row>
-    <row r="72" spans="1:7" ht="16">
+    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -1361,7 +1594,7 @@
       <c r="F72" s="7"/>
       <c r="G72" s="8"/>
     </row>
-    <row r="73" spans="1:7" ht="16">
+    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -1370,7 +1603,7 @@
       <c r="F73" s="7"/>
       <c r="G73" s="8"/>
     </row>
-    <row r="74" spans="1:7" ht="16">
+    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -1379,7 +1612,7 @@
       <c r="F74" s="7"/>
       <c r="G74" s="8"/>
     </row>
-    <row r="75" spans="1:7" ht="16">
+    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -1388,7 +1621,7 @@
       <c r="F75" s="7"/>
       <c r="G75" s="8"/>
     </row>
-    <row r="76" spans="1:7" ht="16">
+    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -1397,7 +1630,7 @@
       <c r="F76" s="7"/>
       <c r="G76" s="8"/>
     </row>
-    <row r="77" spans="1:7" ht="16">
+    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -1406,7 +1639,7 @@
       <c r="F77" s="7"/>
       <c r="G77" s="8"/>
     </row>
-    <row r="78" spans="1:7" ht="16">
+    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -1415,7 +1648,7 @@
       <c r="F78" s="7"/>
       <c r="G78" s="8"/>
     </row>
-    <row r="79" spans="1:7" ht="16">
+    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
@@ -1424,7 +1657,7 @@
       <c r="F79" s="7"/>
       <c r="G79" s="8"/>
     </row>
-    <row r="80" spans="1:7" ht="16">
+    <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -1433,7 +1666,7 @@
       <c r="F80" s="7"/>
       <c r="G80" s="8"/>
     </row>
-    <row r="81" spans="1:7" ht="16">
+    <row r="81" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -1442,7 +1675,7 @@
       <c r="F81" s="7"/>
       <c r="G81" s="8"/>
     </row>
-    <row r="82" spans="1:7" ht="16">
+    <row r="82" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -1451,7 +1684,7 @@
       <c r="F82" s="7"/>
       <c r="G82" s="8"/>
     </row>
-    <row r="83" spans="1:7" ht="16">
+    <row r="83" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -1460,7 +1693,7 @@
       <c r="F83" s="7"/>
       <c r="G83" s="8"/>
     </row>
-    <row r="84" spans="1:7" ht="16">
+    <row r="84" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
@@ -1469,7 +1702,7 @@
       <c r="F84" s="7"/>
       <c r="G84" s="8"/>
     </row>
-    <row r="85" spans="1:7" ht="16">
+    <row r="85" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -1478,7 +1711,7 @@
       <c r="F85" s="7"/>
       <c r="G85" s="8"/>
     </row>
-    <row r="86" spans="1:7" ht="16">
+    <row r="86" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -1487,7 +1720,7 @@
       <c r="F86" s="7"/>
       <c r="G86" s="8"/>
     </row>
-    <row r="87" spans="1:7" ht="16">
+    <row r="87" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
@@ -1496,7 +1729,7 @@
       <c r="F87" s="7"/>
       <c r="G87" s="8"/>
     </row>
-    <row r="88" spans="1:7" ht="16">
+    <row r="88" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
@@ -1505,7 +1738,7 @@
       <c r="F88" s="7"/>
       <c r="G88" s="8"/>
     </row>
-    <row r="89" spans="1:7" ht="16">
+    <row r="89" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -1514,7 +1747,7 @@
       <c r="F89" s="7"/>
       <c r="G89" s="8"/>
     </row>
-    <row r="90" spans="1:7" ht="16">
+    <row r="90" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -1523,7 +1756,7 @@
       <c r="F90" s="7"/>
       <c r="G90" s="8"/>
     </row>
-    <row r="91" spans="1:7" ht="16">
+    <row r="91" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -1532,7 +1765,7 @@
       <c r="F91" s="7"/>
       <c r="G91" s="8"/>
     </row>
-    <row r="92" spans="1:7" ht="16">
+    <row r="92" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -1541,7 +1774,7 @@
       <c r="F92" s="7"/>
       <c r="G92" s="8"/>
     </row>
-    <row r="93" spans="1:7" ht="16">
+    <row r="93" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -1550,7 +1783,7 @@
       <c r="F93" s="7"/>
       <c r="G93" s="8"/>
     </row>
-    <row r="94" spans="1:7" ht="16">
+    <row r="94" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -1559,7 +1792,7 @@
       <c r="F94" s="7"/>
       <c r="G94" s="8"/>
     </row>
-    <row r="95" spans="1:7" ht="16">
+    <row r="95" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -1568,7 +1801,7 @@
       <c r="F95" s="7"/>
       <c r="G95" s="8"/>
     </row>
-    <row r="96" spans="1:7" ht="16">
+    <row r="96" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -1577,7 +1810,7 @@
       <c r="F96" s="7"/>
       <c r="G96" s="8"/>
     </row>
-    <row r="97" spans="1:7" ht="16">
+    <row r="97" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -1586,7 +1819,7 @@
       <c r="F97" s="7"/>
       <c r="G97" s="8"/>
     </row>
-    <row r="98" spans="1:7" ht="16">
+    <row r="98" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
@@ -1595,7 +1828,7 @@
       <c r="F98" s="7"/>
       <c r="G98" s="8"/>
     </row>
-    <row r="99" spans="1:7" ht="16">
+    <row r="99" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -1604,7 +1837,7 @@
       <c r="F99" s="7"/>
       <c r="G99" s="8"/>
     </row>
-    <row r="100" spans="1:7" ht="16">
+    <row r="100" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -1613,7 +1846,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="8"/>
     </row>
-    <row r="101" spans="1:7" ht="16">
+    <row r="101" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -1622,7 +1855,7 @@
       <c r="F101" s="7"/>
       <c r="G101" s="8"/>
     </row>
-    <row r="102" spans="1:7" ht="16">
+    <row r="102" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -1631,7 +1864,7 @@
       <c r="F102" s="7"/>
       <c r="G102" s="8"/>
     </row>
-    <row r="103" spans="1:7" ht="16">
+    <row r="103" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -1640,7 +1873,7 @@
       <c r="F103" s="7"/>
       <c r="G103" s="8"/>
     </row>
-    <row r="104" spans="1:7" ht="16">
+    <row r="104" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -1649,7 +1882,7 @@
       <c r="F104" s="7"/>
       <c r="G104" s="8"/>
     </row>
-    <row r="105" spans="1:7" ht="16">
+    <row r="105" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -1658,7 +1891,7 @@
       <c r="F105" s="7"/>
       <c r="G105" s="8"/>
     </row>
-    <row r="106" spans="1:7" ht="16">
+    <row r="106" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -1667,7 +1900,7 @@
       <c r="F106" s="7"/>
       <c r="G106" s="8"/>
     </row>
-    <row r="107" spans="1:7" ht="16">
+    <row r="107" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -1676,7 +1909,7 @@
       <c r="F107" s="7"/>
       <c r="G107" s="8"/>
     </row>
-    <row r="108" spans="1:7" ht="16">
+    <row r="108" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -1685,7 +1918,7 @@
       <c r="F108" s="7"/>
       <c r="G108" s="8"/>
     </row>
-    <row r="109" spans="1:7" ht="16">
+    <row r="109" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
@@ -1694,7 +1927,7 @@
       <c r="F109" s="7"/>
       <c r="G109" s="8"/>
     </row>
-    <row r="110" spans="1:7" ht="16">
+    <row r="110" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
@@ -1703,7 +1936,7 @@
       <c r="F110" s="7"/>
       <c r="G110" s="8"/>
     </row>
-    <row r="111" spans="1:7" ht="16">
+    <row r="111" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
@@ -1712,7 +1945,7 @@
       <c r="F111" s="7"/>
       <c r="G111" s="8"/>
     </row>
-    <row r="112" spans="1:7" ht="16">
+    <row r="112" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
@@ -1721,7 +1954,7 @@
       <c r="F112" s="7"/>
       <c r="G112" s="8"/>
     </row>
-    <row r="113" spans="1:7" ht="16">
+    <row r="113" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
@@ -1730,7 +1963,7 @@
       <c r="F113" s="7"/>
       <c r="G113" s="8"/>
     </row>
-    <row r="114" spans="1:7" ht="16">
+    <row r="114" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
@@ -1739,7 +1972,7 @@
       <c r="F114" s="7"/>
       <c r="G114" s="8"/>
     </row>
-    <row r="115" spans="1:7" ht="16">
+    <row r="115" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
@@ -1748,7 +1981,7 @@
       <c r="F115" s="7"/>
       <c r="G115" s="8"/>
     </row>
-    <row r="116" spans="1:7" ht="16">
+    <row r="116" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
@@ -1757,7 +1990,7 @@
       <c r="F116" s="7"/>
       <c r="G116" s="8"/>
     </row>
-    <row r="117" spans="1:7" ht="16">
+    <row r="117" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
@@ -1766,7 +1999,7 @@
       <c r="F117" s="7"/>
       <c r="G117" s="8"/>
     </row>
-    <row r="118" spans="1:7" ht="16">
+    <row r="118" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
@@ -1775,7 +2008,7 @@
       <c r="F118" s="7"/>
       <c r="G118" s="8"/>
     </row>
-    <row r="119" spans="1:7" ht="16">
+    <row r="119" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
@@ -1784,7 +2017,7 @@
       <c r="F119" s="7"/>
       <c r="G119" s="8"/>
     </row>
-    <row r="120" spans="1:7" ht="16">
+    <row r="120" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
@@ -1793,7 +2026,7 @@
       <c r="F120" s="7"/>
       <c r="G120" s="8"/>
     </row>
-    <row r="121" spans="1:7" ht="16">
+    <row r="121" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
@@ -1802,7 +2035,7 @@
       <c r="F121" s="7"/>
       <c r="G121" s="8"/>
     </row>
-    <row r="122" spans="1:7" ht="16">
+    <row r="122" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
@@ -1811,7 +2044,7 @@
       <c r="F122" s="7"/>
       <c r="G122" s="8"/>
     </row>
-    <row r="123" spans="1:7" ht="16">
+    <row r="123" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
@@ -1820,7 +2053,7 @@
       <c r="F123" s="7"/>
       <c r="G123" s="8"/>
     </row>
-    <row r="124" spans="1:7" ht="16">
+    <row r="124" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
@@ -1829,7 +2062,7 @@
       <c r="F124" s="7"/>
       <c r="G124" s="8"/>
     </row>
-    <row r="125" spans="1:7" ht="16">
+    <row r="125" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>

</xml_diff>